<commit_message>
survey checkbox bug fixed and new text on register page
</commit_message>
<xml_diff>
--- a/app/static/csv/register.xlsx
+++ b/app/static/csv/register.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\ruchella\agestudy\app\static\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA6A583-D371-422D-852C-01A813938762}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{688290F5-F1DF-4414-8C5F-CCCB9DD1756E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="160">
   <si>
     <t>tag</t>
   </si>
@@ -491,6 +491,15 @@
   </si>
   <si>
     <t>Ik heb een smartphone met Android (geen iPhone)</t>
+  </si>
+  <si>
+    <t>info_icon</t>
+  </si>
+  <si>
+    <t>Once registered please check your email (inbox and spam folders) to activate the App</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zodra u geregistreerd bent: controleer uw e-mail (inbox en eventueel de spam folder) om de App te kunnen activeren. </t>
   </si>
 </sst>
 </file>
@@ -1334,10 +1343,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C60"/>
+  <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="C42" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2007,6 +2016,17 @@
         <v>136</v>
       </c>
     </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>157</v>
+      </c>
+      <c r="B61" t="s">
+        <v>158</v>
+      </c>
+      <c r="C61" t="s">
+        <v>159</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2014,18 +2034,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2207,18 +2227,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9CD5E69-85B0-4DA7-BF73-BF11A37D9D12}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3CCF75A-7D36-4891-89F1-A9732AC92815}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3CCF75A-7D36-4891-89F1-A9732AC92815}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9CD5E69-85B0-4DA7-BF73-BF11A37D9D12}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
errors on register page fixed after rec system release
</commit_message>
<xml_diff>
--- a/app/static/csv/register.xlsx
+++ b/app/static/csv/register.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\ruchella\agestudy\app\static\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EACF5EE-2002-48C9-BBB2-2E9D3DCB1687}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C5D6023-DB32-40AF-B648-BE489C09E4EB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="register" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -515,9 +514,6 @@
     <t>label_promo_code</t>
   </si>
   <si>
-    <t>Has this study been recommended to you by a friend? Fill in their promocode here (optional)</t>
-  </si>
-  <si>
     <t>invalid_feedback_promo_code</t>
   </si>
   <si>
@@ -530,13 +526,16 @@
     <t>valid_feedback_promo_code</t>
   </si>
   <si>
-    <t>Deze code wordt gebruikt om degene die u heeft doorverwezen te belonen. Door de beloning zou hij/zij kunnen zien of u wel of niet de volledige periode deelneemt aan het onderzoek. Verder zullen er geen data van u worden gedeeld met degene die u heeft verwezen.</t>
-  </si>
-  <si>
     <t>The promotion code is used for rewarding your acquaintance and thus he/she may know if you successfully participated or not. No other user data is shared with the acquaintance who gave you this code.</t>
   </si>
   <si>
-    <t>Bent u doorverwezen naar dit onderzoek door een vriend? Vul hier hun promocode in (optioneel)</t>
+    <t xml:space="preserve">Did a friend give you a promocode? (OPTIONAL) </t>
+  </si>
+  <si>
+    <t>Heeft een vriend u een promocode gegeven? (OPTIONEEL)</t>
+  </si>
+  <si>
+    <t>Deze code wordt gebruikt om degene die u heeft doorverwezen te belonen. Door de beloning zou hij/zij kunnen zien of u wel of niet succesvol heeft deelgenomen aan dit onderzoek.</t>
   </si>
 </sst>
 </file>
@@ -1383,7 +1382,7 @@
   <dimension ref="A1:C65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C53" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2080,32 +2079,32 @@
         <v>163</v>
       </c>
       <c r="B63" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="C63" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
+        <v>164</v>
+      </c>
+      <c r="B64" t="s">
         <v>165</v>
       </c>
-      <c r="B64" t="s">
+      <c r="C64" t="s">
         <v>166</v>
-      </c>
-      <c r="C64" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
+        <v>167</v>
+      </c>
+      <c r="B65" t="s">
         <v>168</v>
       </c>
-      <c r="B65" t="s">
-        <v>170</v>
-      </c>
       <c r="C65" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>